<commit_message>
Trying to min violations
</commit_message>
<xml_diff>
--- a/CASE_E_output_A.xlsx
+++ b/CASE_E_output_A.xlsx
@@ -590,27 +590,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -625,32 +625,32 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -660,27 +660,27 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -695,37 +695,37 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -757,7 +757,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -767,7 +767,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -787,17 +787,17 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -822,22 +822,22 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
@@ -852,17 +852,17 @@
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
@@ -872,7 +872,7 @@
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
     </row>
@@ -884,27 +884,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -914,67 +914,67 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -989,27 +989,27 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr">
@@ -1041,12 +1041,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -1081,22 +1081,22 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
@@ -1131,7 +1131,7 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
@@ -1146,7 +1146,7 @@
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
@@ -1161,12 +1161,12 @@
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
     </row>
@@ -1178,132 +1178,132 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AB6" t="inlineStr">
@@ -1330,22 +1330,22 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1360,27 +1360,27 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -1390,7 +1390,7 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1400,17 +1400,17 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
@@ -1430,17 +1430,17 @@
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
@@ -1455,7 +1455,7 @@
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr">
@@ -1472,117 +1472,117 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
@@ -1597,17 +1597,17 @@
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
     </row>
@@ -1629,22 +1629,22 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1664,17 +1664,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1689,37 +1689,37 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
@@ -1734,17 +1734,17 @@
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AB9" t="inlineStr">
@@ -1754,7 +1754,7 @@
       </c>
       <c r="AC9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1776,17 +1776,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1811,17 +1811,17 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1831,32 +1831,32 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -1871,7 +1871,7 @@
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
@@ -1881,17 +1881,17 @@
       </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AB10" t="inlineStr">
@@ -1913,17 +1913,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1943,7 +1943,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1953,12 +1953,12 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1973,7 +1973,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
@@ -1983,17 +1983,17 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
@@ -2008,12 +2008,12 @@
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
@@ -2023,12 +2023,12 @@
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Z11" t="inlineStr">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AB11" t="inlineStr">
@@ -2085,12 +2085,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -2100,27 +2100,27 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
@@ -2135,37 +2135,37 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
@@ -2175,27 +2175,27 @@
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2207,12 +2207,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -2227,17 +2227,17 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -2262,17 +2262,17 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -2282,67 +2282,67 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AC13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2359,47 +2359,47 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -2409,52 +2409,52 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
@@ -2474,22 +2474,22 @@
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AC14" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2501,12 +2501,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -2521,12 +2521,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -2536,12 +2536,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -2551,17 +2551,17 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -2571,12 +2571,12 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -2586,32 +2586,32 @@
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
@@ -2621,12 +2621,12 @@
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AB15" t="inlineStr">
@@ -2636,7 +2636,7 @@
       </c>
       <c r="AC15" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2653,7 +2653,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -2663,27 +2663,27 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -2698,22 +2698,22 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -2728,42 +2728,42 @@
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Z16" t="inlineStr">
@@ -2778,12 +2778,12 @@
       </c>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AC16" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2795,57 +2795,57 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -2855,12 +2855,12 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -2870,7 +2870,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -2880,7 +2880,7 @@
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
@@ -2890,7 +2890,7 @@
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
@@ -2900,7 +2900,7 @@
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
@@ -2910,22 +2910,22 @@
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AC17" t="inlineStr">
@@ -2942,12 +2942,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2957,27 +2957,27 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -2987,7 +2987,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -3002,7 +3002,7 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
@@ -3022,62 +3022,62 @@
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC18" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -3089,17 +3089,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -3119,7 +3119,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -3129,37 +3129,37 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
@@ -3174,57 +3174,57 @@
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC19" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
     </row>
@@ -3241,117 +3241,117 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="Z20" t="inlineStr">
@@ -3361,17 +3361,17 @@
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AC20" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
     </row>
@@ -3383,12 +3383,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -3398,32 +3398,32 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -3448,7 +3448,7 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -3458,42 +3458,42 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="Y21" t="inlineStr">
@@ -3503,22 +3503,22 @@
       </c>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AC21" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -3530,37 +3530,37 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -3585,52 +3585,52 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
@@ -3645,22 +3645,22 @@
       </c>
       <c r="Y22" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AC22" t="inlineStr">
@@ -3677,7 +3677,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -3687,17 +3687,17 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -3712,12 +3712,12 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -3732,57 +3732,57 @@
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="W23" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="X23" t="inlineStr">
@@ -3792,22 +3792,22 @@
       </c>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AB23" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AC23" t="inlineStr">
@@ -3824,32 +3824,32 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -3859,42 +3859,42 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
@@ -3904,12 +3904,12 @@
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="T24" t="inlineStr">
@@ -3924,27 +3924,27 @@
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AA24" t="inlineStr">
@@ -3959,7 +3959,7 @@
       </c>
       <c r="AC24" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
     </row>
@@ -3971,22 +3971,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3996,47 +3996,47 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -4051,62 +4051,62 @@
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="W25" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AC25" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -4133,27 +4133,27 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -4168,22 +4168,22 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -4203,57 +4203,57 @@
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="W26" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AB26" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC26" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
     </row>
@@ -4265,22 +4265,22 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -4290,12 +4290,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -4305,7 +4305,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -4315,7 +4315,7 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
@@ -4325,22 +4325,22 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -4370,22 +4370,22 @@
       </c>
       <c r="W27" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AA27" t="inlineStr">
@@ -4395,12 +4395,12 @@
       </c>
       <c r="AB27" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AC27" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
     </row>
@@ -4412,7 +4412,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -4422,27 +4422,27 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -4452,17 +4452,17 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -4477,12 +4477,12 @@
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
@@ -4492,12 +4492,12 @@
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="T28" t="inlineStr">
@@ -4507,12 +4507,12 @@
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="W28" t="inlineStr">
@@ -4537,12 +4537,12 @@
       </c>
       <c r="AA28" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AB28" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AC28" t="inlineStr">
@@ -4559,32 +4559,32 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -4594,12 +4594,12 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -4619,37 +4619,37 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="T29" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="U29" t="inlineStr">
@@ -4659,42 +4659,42 @@
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="W29" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AA29" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AB29" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AC29" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -4706,12 +4706,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -4726,42 +4726,42 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
@@ -4776,17 +4776,17 @@
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
@@ -4796,27 +4796,27 @@
       </c>
       <c r="T30" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="U30" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="W30" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
@@ -4836,12 +4836,12 @@
       </c>
       <c r="AB30" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC30" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
     </row>
@@ -4853,7 +4853,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -4863,32 +4863,32 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -4903,12 +4903,12 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
@@ -4918,17 +4918,17 @@
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -4943,7 +4943,7 @@
       </c>
       <c r="T31" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="U31" t="inlineStr">
@@ -4953,22 +4953,22 @@
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="W31" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="Z31" t="inlineStr">
@@ -4978,7 +4978,7 @@
       </c>
       <c r="AA31" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AB31" t="inlineStr">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="AC31" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -5005,12 +5005,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -5020,42 +5020,42 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
@@ -5065,17 +5065,17 @@
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -5085,32 +5085,32 @@
       </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="T32" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="W32" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
@@ -5120,22 +5120,22 @@
       </c>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AA32" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AB32" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="AC32" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
     </row>
@@ -5147,32 +5147,32 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -5187,7 +5187,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -5212,7 +5212,7 @@
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -5222,42 +5222,42 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>N</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="T33" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>L</t>
         </is>
       </c>
       <c r="W33" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
@@ -5267,17 +5267,17 @@
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>E</t>
         </is>
       </c>
       <c r="AA33" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AB33" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC33" t="inlineStr">
@@ -5334,13 +5334,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>33649</v>
+        <v>34980</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>

</xml_diff>